<commit_message>
files to be translated updates
</commit_message>
<xml_diff>
--- a/measures/awareness_2c.xlsx
+++ b/measures/awareness_2c.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/unconscious-ec-RRR/measures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6834889-13AC-A741-8630-8A7683463631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="460" windowWidth="26820" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="2240" windowWidth="26820" windowHeight="17040"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -638,7 +637,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -690,7 +689,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -884,31 +883,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="89.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="231" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="231" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -916,5 +913,10 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>